<commit_message>
Snapshot of Raw Data Files Captured
</commit_message>
<xml_diff>
--- a/IPEDSData_Raw.xlsx
+++ b/IPEDSData_Raw.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nwmissouri-my.sharepoint.com/personal/meghaan_nwmissouri_edu/Documents/44-688/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nwmissouri-my.sharepoint.com/personal/meghaan_nwmissouri_edu/Documents/44-688/M.S.-Data-Analytics-Capstone-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CAB0D83F-7C2D-4DE0-A26F-EFBF9CA2C023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{CAB0D83F-7C2D-4DE0-A26F-EFBF9CA2C023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D8CC3AD-A1C1-4AAF-ACDF-55B14825E843}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11235"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IPEDS Data 3-13-24" sheetId="1" r:id="rId1"/>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -937,12 +937,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.42578125" customWidth="1"/>
+    <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>